<commit_message>
changes in the other excels
</commit_message>
<xml_diff>
--- a/src/test/resources/testDuplicate.xlsx
+++ b/src/test/resources/testDuplicate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
@@ -35,9 +35,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Localización</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
@@ -50,7 +47,10 @@
     <t>59687412O</t>
   </si>
   <si>
-    <t>36S78W</t>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
   </si>
 </sst>
 </file>
@@ -413,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,43 +432,52 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>15.56</v>
+      </c>
+      <c r="E2">
+        <v>25.26</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="D3">
+        <v>15.56</v>
       </c>
       <c r="E3">
+        <v>25.26</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
     </row>

</xml_diff>